<commit_message>
Commit with both main and test code
</commit_message>
<xml_diff>
--- a/src/test/resources/Testdata/Contacts.xlsx.xlsx
+++ b/src/test/resources/Testdata/Contacts.xlsx.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/316509db2eef755f/Documents/Custom Office Templates/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Java Program\ContactManagement\src\test\resources\Testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5C308A28-9710-4DF9-B3D5-29DD3DB55019}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{823D45CD-9E80-4BFE-8EF9-7DEE18BC1339}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{0F4B02C6-27A0-4F5B-83E6-BBA097C6FA20}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="1" xr2:uid="{0F4B02C6-27A0-4F5B-83E6-BBA097C6FA20}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Login Data" sheetId="1" r:id="rId1"/>
+    <sheet name="Signup Data" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,89 +35,94 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
-  <si>
-    <t>Last Name</t>
-  </si>
-  <si>
-    <t>DOB</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="24">
   <si>
     <t>Email</t>
   </si>
   <si>
-    <t>Phone</t>
-  </si>
-  <si>
-    <t>Street</t>
-  </si>
-  <si>
-    <t>City</t>
-  </si>
-  <si>
-    <t>State</t>
-  </si>
-  <si>
-    <t>Pincode</t>
-  </si>
-  <si>
-    <t>Country</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ravi   </t>
-  </si>
-  <si>
     <t>Kumar</t>
   </si>
   <si>
-    <t>ravi.k@example.com</t>
-  </si>
-  <si>
-    <t>123 Main St</t>
-  </si>
-  <si>
-    <t>Chennai</t>
-  </si>
-  <si>
-    <t>TN</t>
-  </si>
-  <si>
-    <t>India</t>
-  </si>
-  <si>
     <t>FirstName</t>
   </si>
   <si>
-    <t xml:space="preserve">Priya   </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sharma </t>
-  </si>
-  <si>
-    <t xml:space="preserve">   1988-11-15</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> priya.s@example.com  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">456 Park Ln   </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bangalore </t>
-  </si>
-  <si>
-    <t xml:space="preserve">KA    </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> India</t>
+    <t>TestCase</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>ExpectedResult</t>
+  </si>
+  <si>
+    <t>ValidLogin</t>
+  </si>
+  <si>
+    <t>cdkarvendhan@gmail.com</t>
+  </si>
+  <si>
+    <t>ValidPass123</t>
+  </si>
+  <si>
+    <t>Success</t>
+  </si>
+  <si>
+    <t>InvalidPassword</t>
+  </si>
+  <si>
+    <t>WrongPass123</t>
+  </si>
+  <si>
+    <t>Error</t>
+  </si>
+  <si>
+    <t>EmptyFields</t>
+  </si>
+  <si>
+    <t>InvalidEmailFormat</t>
+  </si>
+  <si>
+    <t>invalidemail@</t>
+  </si>
+  <si>
+    <t>LastName</t>
+  </si>
+  <si>
+    <t>ValidSignup</t>
+  </si>
+  <si>
+    <t>Ravi</t>
+  </si>
+  <si>
+    <t>random@example.com</t>
+  </si>
+  <si>
+    <t>ExistingEmail</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>User</t>
+  </si>
+  <si>
+    <t>invalid-email</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -144,13 +150,25 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -466,116 +484,200 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51EE9545-2A15-4FFE-801D-B732D656D4B1}">
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J21" sqref="J21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.33203125" customWidth="1"/>
-    <col min="2" max="2" width="12.44140625" customWidth="1"/>
+    <col min="1" max="1" width="18.5546875" customWidth="1"/>
+    <col min="2" max="2" width="28.44140625" customWidth="1"/>
     <col min="3" max="3" width="15.109375" customWidth="1"/>
     <col min="4" max="4" width="25.21875" customWidth="1"/>
     <col min="5" max="5" width="16.44140625" customWidth="1"/>
     <col min="6" max="6" width="11.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7AFDD033-940C-475E-9CB8-8A324D75EC63}">
+  <dimension ref="A1:F5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="20" customWidth="1"/>
+    <col min="2" max="3" width="18" customWidth="1"/>
+    <col min="4" max="4" width="21.33203125" customWidth="1"/>
+    <col min="5" max="5" width="19.21875" customWidth="1"/>
+    <col min="6" max="6" width="13.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" s="2" t="s">
+      <c r="D2" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="E3" s="3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" s="1">
-        <v>33013</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" s="2">
-        <v>9876543210</v>
-      </c>
-      <c r="F2" s="2" t="s">
+      <c r="F3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="2" t="s">
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="I2" s="2">
-        <v>600001</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E3" s="2">
-        <v>8765432109</v>
-      </c>
-      <c r="F3" s="2" t="s">
+      <c r="B5" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="C5" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="D5" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="I3" s="2">
-        <v>560001</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>24</v>
+      <c r="E5" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>